<commit_message>
Added top right corner purple cell with a number
</commit_message>
<xml_diff>
--- a/dptos v1.xlsx
+++ b/dptos v1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AB84\First-Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A66CE8AA-B9CF-4623-99A0-56C532ED9D82}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F60E5C89-98F2-40BA-9F2E-C3759F0CD438}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{AC42E626-5A29-4158-A6DB-462C3042FB4C}"/>
   </bookViews>
@@ -378,9 +378,6 @@
     <t>https://www.portalinmobiliario.com/arriendo/departamento/vitacura-metropolitana/5874006-vitacura-las-tranqueras-uda</t>
   </si>
   <si>
-    <t>Estadio Croata</t>
-  </si>
-  <si>
     <t>Escuela militar (metro)</t>
   </si>
   <si>
@@ -680,6 +677,9 @@
   </si>
   <si>
     <t>Suecia, Los Leones, Providencia</t>
+  </si>
+  <si>
+    <t>Estadio Croata (muebles feos)</t>
   </si>
 </sst>
 </file>
@@ -748,7 +748,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -800,6 +800,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -863,7 +869,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -928,6 +934,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1261,7 +1268,7 @@
       <pane xSplit="8" ySplit="3" topLeftCell="I4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E12" sqref="E12"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1288,36 +1295,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="19"/>
+      <c r="A1" s="34">
+        <v>555</v>
+      </c>
       <c r="B1" s="19"/>
       <c r="C1" s="19"/>
       <c r="D1" s="20"/>
       <c r="E1" s="19"/>
       <c r="F1" s="19"/>
       <c r="G1" s="23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H1" s="23"/>
       <c r="I1" s="23"/>
       <c r="J1" s="23"/>
       <c r="K1" s="23"/>
       <c r="L1" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="M1" s="25"/>
       <c r="N1" s="26"/>
       <c r="O1" s="27" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="P1" s="27"/>
       <c r="Q1" s="28"/>
       <c r="R1" s="28"/>
       <c r="S1" s="29" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="T1" s="31"/>
       <c r="U1" s="23" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="V1" s="23"/>
       <c r="W1" s="23"/>
@@ -1328,16 +1337,16 @@
       <c r="AB1" s="23"/>
       <c r="AC1" s="23"/>
       <c r="AD1" s="24" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="AE1" s="24"/>
       <c r="AI1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:35" ht="90" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>1</v>
@@ -1352,10 +1361,10 @@
         <v>0</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>2</v>
@@ -1367,65 +1376,65 @@
         <v>4</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L2" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="M2" s="4" t="s">
         <v>9</v>
       </c>
       <c r="N2" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="O2" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="P2" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="O2" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="P2" s="16" t="s">
+      <c r="Q2" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="S2" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="T2" s="30" t="s">
         <v>85</v>
       </c>
-      <c r="Q2" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="R2" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="S2" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="T2" s="30" t="s">
-        <v>86</v>
-      </c>
       <c r="U2" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="V2" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="V2" s="4" t="s">
+      <c r="W2" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="W2" s="4" t="s">
+      <c r="X2" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="X2" s="4" t="s">
+      <c r="Y2" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="Y2" s="4" t="s">
+      <c r="Z2" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="Z2" s="4" t="s">
+      <c r="AA2" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="AA2" s="4" t="s">
+      <c r="AB2" s="4" t="s">
         <v>104</v>
-      </c>
-      <c r="AB2" s="4" t="s">
-        <v>105</v>
       </c>
       <c r="AC2" s="4"/>
       <c r="AD2" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AE2" s="16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="AF2" s="4" t="s">
         <v>5</v>
@@ -1434,7 +1443,7 @@
         <v>7</v>
       </c>
       <c r="AH2" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AI2" s="4" t="s">
         <v>6</v>
@@ -1472,11 +1481,11 @@
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A4" s="10">
-        <f>A3+1</f>
+        <f t="shared" ref="A4:A38" si="0">A3+1</f>
         <v>1</v>
       </c>
       <c r="B4" s="32" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C4" s="5">
         <v>2</v>
@@ -1485,7 +1494,7 @@
         <v>2</v>
       </c>
       <c r="E4" s="5">
-        <f>IF(G4&lt;&gt;"",G4,F4)</f>
+        <f t="shared" ref="E4:E38" si="1">IF(G4&lt;&gt;"",G4,F4)</f>
         <v>61</v>
       </c>
       <c r="F4" s="5">
@@ -1501,11 +1510,11 @@
         <v>100</v>
       </c>
       <c r="J4" s="5">
-        <f>H4+I4</f>
+        <f t="shared" ref="J4:J35" si="2">H4+I4</f>
         <v>550</v>
       </c>
       <c r="K4" s="2">
-        <f>J4/E4</f>
+        <f t="shared" ref="K4:K38" si="3">J4/E4</f>
         <v>9.0163934426229506</v>
       </c>
       <c r="L4" s="13">
@@ -1515,14 +1524,14 @@
         <v>2</v>
       </c>
       <c r="N4" s="17">
-        <f>IF(L4&lt;1,(J4+$B$49)/E4,K4)</f>
+        <f t="shared" ref="N4:N38" si="4">IF(L4&lt;1,(J4+$B$49)/E4,K4)</f>
         <v>9.0163934426229506</v>
       </c>
       <c r="O4">
         <v>1</v>
       </c>
       <c r="P4" s="17">
-        <f>(J4
+        <f t="shared" ref="P4:P38" si="5">(J4
 +(IF(L4&lt;1,esta,0)
 +(O4-1)*amob))
 /E4</f>
@@ -1533,7 +1542,7 @@
         <v>2</v>
       </c>
       <c r="T4" s="17">
-        <f>(J4
+        <f t="shared" ref="T4:T38" si="6">(J4
 +(IF(L4&lt;1,esta,0)
 +(O4-1)*amob)
 +(S4-1)*este)
@@ -1551,18 +1560,18 @@
       <c r="AC4" s="6"/>
       <c r="AD4" s="13"/>
       <c r="AF4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AG4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AI4" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A5" s="10">
-        <f>A4+1</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="B5" s="7" t="s">
@@ -1575,7 +1584,7 @@
         <v>1</v>
       </c>
       <c r="E5" s="5">
-        <f>IF(G5&lt;&gt;"",G5,F5)</f>
+        <f t="shared" si="1"/>
         <v>60</v>
       </c>
       <c r="F5" s="5">
@@ -1591,11 +1600,11 @@
         <v>65</v>
       </c>
       <c r="J5" s="5">
-        <f>H5+I5</f>
+        <f t="shared" si="2"/>
         <v>485</v>
       </c>
       <c r="K5" s="2">
-        <f>J5/E5</f>
+        <f t="shared" si="3"/>
         <v>8.0833333333333339</v>
       </c>
       <c r="L5" s="13">
@@ -1605,17 +1614,14 @@
         <v>1</v>
       </c>
       <c r="N5" s="17">
-        <f>IF(L5&lt;1,(J5+$B$49)/E5,K5)</f>
+        <f t="shared" si="4"/>
         <v>8.0833333333333339</v>
       </c>
       <c r="O5">
         <v>2</v>
       </c>
       <c r="P5" s="17">
-        <f>(J5
-+(IF(L5&lt;1,esta,0)
-+(O5-1)*amob))
-/E5</f>
+        <f t="shared" si="5"/>
         <v>8.6388888888888893</v>
       </c>
       <c r="Q5" s="5"/>
@@ -1623,11 +1629,7 @@
         <v>3</v>
       </c>
       <c r="T5" s="17">
-        <f>(J5
-+(IF(L5&lt;1,esta,0)
-+(O5-1)*amob)
-+(S5-1)*este)
-/E5</f>
+        <f t="shared" si="6"/>
         <v>9.4722222222222232</v>
       </c>
       <c r="U5" s="6"/>
@@ -1644,7 +1646,7 @@
         <v>17</v>
       </c>
       <c r="AG5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AI5" s="1" t="s">
         <v>13</v>
@@ -1652,7 +1654,7 @@
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A6" s="10">
-        <f>A5+1</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="B6" s="32" t="s">
@@ -1665,7 +1667,7 @@
         <v>1</v>
       </c>
       <c r="E6" s="5">
-        <f>IF(G6&lt;&gt;"",G6,F6)</f>
+        <f t="shared" si="1"/>
         <v>58</v>
       </c>
       <c r="F6" s="5">
@@ -1681,11 +1683,11 @@
         <v>100</v>
       </c>
       <c r="J6" s="5">
-        <f>H6+I6</f>
+        <f t="shared" si="2"/>
         <v>530</v>
       </c>
       <c r="K6" s="2">
-        <f>J6/E6</f>
+        <f t="shared" si="3"/>
         <v>9.137931034482758</v>
       </c>
       <c r="L6" s="13">
@@ -1695,17 +1697,14 @@
         <v>0</v>
       </c>
       <c r="N6" s="17">
-        <f>IF(L6&lt;1,(J6+$B$49)/E6,K6)</f>
+        <f t="shared" si="4"/>
         <v>9.137931034482758</v>
       </c>
       <c r="O6">
         <v>1</v>
       </c>
       <c r="P6" s="17">
-        <f>(J6
-+(IF(L6&lt;1,esta,0)
-+(O6-1)*amob))
-/E6</f>
+        <f t="shared" si="5"/>
         <v>9.137931034482758</v>
       </c>
       <c r="Q6" s="5"/>
@@ -1716,43 +1715,39 @@
         <v>2</v>
       </c>
       <c r="T6" s="17">
-        <f>(J6
-+(IF(L6&lt;1,esta,0)
-+(O6-1)*amob)
-+(S6-1)*este)
-/E6</f>
+        <f t="shared" si="6"/>
         <v>9.568965517241379</v>
       </c>
       <c r="U6" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="V6" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="W6" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="X6" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="Y6" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="Z6" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="AA6" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="AB6" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="AC6" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="AD6" s="13"/>
       <c r="AG6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AI6" s="1" t="s">
         <v>22</v>
@@ -1760,11 +1755,11 @@
     </row>
     <row r="7" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A7" s="10">
-        <f>A6+1</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C7" s="5">
         <v>1</v>
@@ -1773,7 +1768,7 @@
         <v>1</v>
       </c>
       <c r="E7" s="5">
-        <f>IF(G7&lt;&gt;"",G7,F7)</f>
+        <f t="shared" si="1"/>
         <v>55</v>
       </c>
       <c r="F7" s="5">
@@ -1789,11 +1784,11 @@
         <v>100</v>
       </c>
       <c r="J7" s="5">
-        <f>H7+I7</f>
+        <f t="shared" si="2"/>
         <v>520</v>
       </c>
       <c r="K7" s="2">
-        <f>J7/E7</f>
+        <f t="shared" si="3"/>
         <v>9.454545454545455</v>
       </c>
       <c r="L7" s="13">
@@ -1803,17 +1798,14 @@
         <v>0</v>
       </c>
       <c r="N7" s="17">
-        <f>IF(L7&lt;1,(J7+$B$49)/E7,K7)</f>
+        <f t="shared" si="4"/>
         <v>9.454545454545455</v>
       </c>
       <c r="O7">
         <v>1</v>
       </c>
       <c r="P7" s="17">
-        <f>(J7
-+(IF(L7&lt;1,esta,0)
-+(O7-1)*amob))
-/E7</f>
+        <f t="shared" si="5"/>
         <v>9.454545454545455</v>
       </c>
       <c r="Q7" s="5"/>
@@ -1821,11 +1813,7 @@
         <v>4</v>
       </c>
       <c r="T7" s="17">
-        <f>(J7
-+(IF(L7&lt;1,esta,0)
-+(O7-1)*amob)
-+(S7-1)*este)
-/E7</f>
+        <f t="shared" si="6"/>
         <v>10.818181818181818</v>
       </c>
       <c r="U7" s="6"/>
@@ -1839,19 +1827,19 @@
       <c r="AC7" s="6"/>
       <c r="AD7" s="13"/>
       <c r="AG7" t="s">
+        <v>66</v>
+      </c>
+      <c r="AI7" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="AI7" s="1" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A8" s="10">
-        <f>A7+1</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B8" s="32" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C8" s="5">
         <v>1</v>
@@ -1860,7 +1848,7 @@
         <v>1</v>
       </c>
       <c r="E8" s="5">
-        <f>IF(G8&lt;&gt;"",G8,F8)</f>
+        <f t="shared" si="1"/>
         <v>46</v>
       </c>
       <c r="F8" s="5">
@@ -1876,11 +1864,11 @@
         <v>50</v>
       </c>
       <c r="J8" s="5">
-        <f>H8+I8</f>
+        <f t="shared" si="2"/>
         <v>500</v>
       </c>
       <c r="K8" s="2">
-        <f>J8/E8</f>
+        <f t="shared" si="3"/>
         <v>10.869565217391305</v>
       </c>
       <c r="L8" s="13">
@@ -1890,17 +1878,14 @@
         <v>1</v>
       </c>
       <c r="N8" s="17">
-        <f>IF(L8&lt;1,(J8+$B$49)/E8,K8)</f>
+        <f t="shared" si="4"/>
         <v>10.869565217391305</v>
       </c>
       <c r="O8">
         <v>1</v>
       </c>
       <c r="P8" s="17">
-        <f>(J8
-+(IF(L8&lt;1,esta,0)
-+(O8-1)*amob))
-/E8</f>
+        <f t="shared" si="5"/>
         <v>10.869565217391305</v>
       </c>
       <c r="Q8" s="5">
@@ -1910,11 +1895,7 @@
         <v>1</v>
       </c>
       <c r="T8" s="17">
-        <f>(J8
-+(IF(L8&lt;1,esta,0)
-+(O8-1)*amob)
-+(S8-1)*este)
-/E8</f>
+        <f t="shared" si="6"/>
         <v>10.869565217391305</v>
       </c>
       <c r="U8" s="6"/>
@@ -1928,23 +1909,23 @@
       <c r="AC8" s="6"/>
       <c r="AD8" s="13"/>
       <c r="AF8" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AG8" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AH8" s="5"/>
       <c r="AI8" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A9" s="10">
-        <f>A8+1</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B9" s="32" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C9" s="7">
         <v>1</v>
@@ -1953,7 +1934,7 @@
         <v>1</v>
       </c>
       <c r="E9" s="7">
-        <f>IF(G9&lt;&gt;"",G9,F9)</f>
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
       <c r="F9" s="7">
@@ -1969,11 +1950,11 @@
         <v>70</v>
       </c>
       <c r="J9" s="7">
-        <f>H9+I9</f>
+        <f t="shared" si="2"/>
         <v>520</v>
       </c>
       <c r="K9" s="8">
-        <f>J9/E9</f>
+        <f t="shared" si="3"/>
         <v>10.4</v>
       </c>
       <c r="L9" s="13">
@@ -1983,17 +1964,14 @@
         <v>1</v>
       </c>
       <c r="N9" s="21">
-        <f>IF(L9&lt;1,(J9+$B$49)/E9,K9)</f>
+        <f t="shared" si="4"/>
         <v>10.4</v>
       </c>
       <c r="O9">
         <v>1</v>
       </c>
       <c r="P9" s="17">
-        <f>(J9
-+(IF(L9&lt;1,esta,0)
-+(O9-1)*amob))
-/E9</f>
+        <f t="shared" si="5"/>
         <v>10.4</v>
       </c>
       <c r="R9">
@@ -2003,31 +1981,27 @@
         <v>2</v>
       </c>
       <c r="T9" s="17">
-        <f>(J9
-+(IF(L9&lt;1,esta,0)
-+(O9-1)*amob)
-+(S9-1)*este)
-/E9</f>
+        <f t="shared" si="6"/>
         <v>10.9</v>
       </c>
       <c r="AD9" s="13"/>
       <c r="AG9" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AH9" t="s">
+        <v>114</v>
+      </c>
+      <c r="AI9" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="AI9" s="1" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A10" s="10">
-        <f>A9+1</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>28</v>
+        <v>124</v>
       </c>
       <c r="C10" s="5">
         <v>2</v>
@@ -2036,7 +2010,7 @@
         <v>2</v>
       </c>
       <c r="E10" s="5">
-        <f>IF(G10&lt;&gt;"",G10,F10)</f>
+        <f t="shared" si="1"/>
         <v>60</v>
       </c>
       <c r="F10" s="5">
@@ -2052,11 +2026,11 @@
         <v>70</v>
       </c>
       <c r="J10" s="5">
-        <f>H10+I10</f>
+        <f t="shared" si="2"/>
         <v>520</v>
       </c>
       <c r="K10" s="2">
-        <f>J10/E10</f>
+        <f t="shared" si="3"/>
         <v>8.6666666666666661</v>
       </c>
       <c r="L10" s="13">
@@ -2066,17 +2040,14 @@
         <v>0</v>
       </c>
       <c r="N10" s="17">
-        <f>IF(L10&lt;1,(J10+$B$49)/E10,K10)</f>
+        <f t="shared" si="4"/>
         <v>9.6666666666666661</v>
       </c>
       <c r="O10">
         <v>1</v>
       </c>
       <c r="P10" s="17">
-        <f>(J10
-+(IF(L10&lt;1,esta,0)
-+(O10-1)*amob))
-/E10</f>
+        <f t="shared" si="5"/>
         <v>9.6666666666666661</v>
       </c>
       <c r="Q10" s="5"/>
@@ -2084,43 +2055,39 @@
         <v>4</v>
       </c>
       <c r="T10" s="17">
-        <f>(J10
-+(IF(L10&lt;1,esta,0)
-+(O10-1)*amob)
-+(S10-1)*este)
-/E10</f>
+        <f t="shared" si="6"/>
         <v>10.916666666666666</v>
       </c>
       <c r="U10" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="V10" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="W10" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="X10" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="Y10" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="Z10" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="AA10" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="AB10" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="AC10" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="AD10" s="13"/>
       <c r="AG10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AI10" s="1" t="s">
         <v>27</v>
@@ -2128,11 +2095,11 @@
     </row>
     <row r="11" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A11" s="10">
-        <f>A10+1</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B11" s="32" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C11" s="5">
         <v>1</v>
@@ -2141,7 +2108,7 @@
         <v>1</v>
       </c>
       <c r="E11" s="5">
-        <f>IF(G11&lt;&gt;"",G11,F11)</f>
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
       <c r="F11" s="5">
@@ -2157,11 +2124,11 @@
         <v>80</v>
       </c>
       <c r="J11" s="5">
-        <f>H11+I11</f>
+        <f t="shared" si="2"/>
         <v>440</v>
       </c>
       <c r="K11" s="2">
-        <f>J11/E11</f>
+        <f t="shared" si="3"/>
         <v>8.8000000000000007</v>
       </c>
       <c r="L11" s="13">
@@ -2171,17 +2138,14 @@
         <v>1</v>
       </c>
       <c r="N11" s="17">
-        <f>IF(L11&lt;1,(J11+$B$49)/E11,K11)</f>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="O11">
         <v>1</v>
       </c>
       <c r="P11" s="17">
-        <f>(J11
-+(IF(L11&lt;1,esta,0)
-+(O11-1)*amob))
-/E11</f>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="Q11" s="5"/>
@@ -2189,11 +2153,7 @@
         <v>3</v>
       </c>
       <c r="T11" s="17">
-        <f>(J11
-+(IF(L11&lt;1,esta,0)
-+(O11-1)*amob)
-+(S11-1)*este)
-/E11</f>
+        <f t="shared" si="6"/>
         <v>11</v>
       </c>
       <c r="U11" s="6"/>
@@ -2207,22 +2167,22 @@
       <c r="AC11" s="6"/>
       <c r="AD11" s="13"/>
       <c r="AG11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AH11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="AI11" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A12" s="10">
-        <f>A11+1</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C12" s="5">
         <v>1</v>
@@ -2231,7 +2191,7 @@
         <v>1</v>
       </c>
       <c r="E12" s="5">
-        <f>IF(G12&lt;&gt;"",G12,F12)</f>
+        <f t="shared" si="1"/>
         <v>60</v>
       </c>
       <c r="F12" s="5">
@@ -2247,11 +2207,11 @@
         <v>60</v>
       </c>
       <c r="J12" s="5">
-        <f>H12+I12</f>
+        <f t="shared" si="2"/>
         <v>510</v>
       </c>
       <c r="K12" s="2">
-        <f>J12/E12</f>
+        <f t="shared" si="3"/>
         <v>8.5</v>
       </c>
       <c r="L12" s="13">
@@ -2261,17 +2221,14 @@
         <v>0</v>
       </c>
       <c r="N12" s="17">
-        <f>IF(L12&lt;1,(J12+$B$49)/E12,K12)</f>
+        <f t="shared" si="4"/>
         <v>9.5</v>
       </c>
       <c r="O12">
         <v>1</v>
       </c>
       <c r="P12" s="17">
-        <f>(J12
-+(IF(L12&lt;1,esta,0)
-+(O12-1)*amob))
-/E12</f>
+        <f t="shared" si="5"/>
         <v>9.5</v>
       </c>
       <c r="Q12" s="5"/>
@@ -2279,11 +2236,7 @@
         <v>5</v>
       </c>
       <c r="T12" s="17">
-        <f>(J12
-+(IF(L12&lt;1,esta,0)
-+(O12-1)*amob)
-+(S12-1)*este)
-/E12</f>
+        <f t="shared" si="6"/>
         <v>11.166666666666666</v>
       </c>
       <c r="U12" s="6"/>
@@ -2297,22 +2250,22 @@
       <c r="AC12" s="6"/>
       <c r="AD12" s="13"/>
       <c r="AF12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AG12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AI12" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A13" s="10">
-        <f>A12+1</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="B13" s="33" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -2321,7 +2274,7 @@
         <v>1</v>
       </c>
       <c r="E13">
-        <f>IF(G13&lt;&gt;"",G13,F13)</f>
+        <f t="shared" si="1"/>
         <v>47</v>
       </c>
       <c r="F13">
@@ -2337,11 +2290,11 @@
         <v>58</v>
       </c>
       <c r="J13">
-        <f>H13+I13</f>
+        <f t="shared" si="2"/>
         <v>478</v>
       </c>
       <c r="K13" s="2">
-        <f>J13/E13</f>
+        <f t="shared" si="3"/>
         <v>10.170212765957446</v>
       </c>
       <c r="L13" s="13">
@@ -2351,17 +2304,14 @@
         <v>1</v>
       </c>
       <c r="N13" s="17">
-        <f>IF(L13&lt;1,(J13+$B$49)/E13,K13)</f>
+        <f t="shared" si="4"/>
         <v>10.170212765957446</v>
       </c>
       <c r="O13">
         <v>1</v>
       </c>
       <c r="P13" s="17">
-        <f>(J13
-+(IF(L13&lt;1,esta,0)
-+(O13-1)*amob))
-/E13</f>
+        <f t="shared" si="5"/>
         <v>10.170212765957446</v>
       </c>
       <c r="Q13" s="5"/>
@@ -2369,11 +2319,7 @@
         <v>3</v>
       </c>
       <c r="T13" s="17">
-        <f>(J13
-+(IF(L13&lt;1,esta,0)
-+(O13-1)*amob)
-+(S13-1)*este)
-/E13</f>
+        <f t="shared" si="6"/>
         <v>11.23404255319149</v>
       </c>
       <c r="U13" s="6"/>
@@ -2387,22 +2333,22 @@
       <c r="AC13" s="6"/>
       <c r="AD13" s="13"/>
       <c r="AG13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AH13" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="AI13" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A14" s="10">
-        <f>A13+1</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -2411,7 +2357,7 @@
         <v>1</v>
       </c>
       <c r="E14">
-        <f>IF(G14&lt;&gt;"",G14,F14)</f>
+        <f t="shared" si="1"/>
         <v>48</v>
       </c>
       <c r="F14">
@@ -2427,11 +2373,11 @@
         <v>90</v>
       </c>
       <c r="J14">
-        <f>H14+I14</f>
+        <f t="shared" si="2"/>
         <v>520</v>
       </c>
       <c r="K14" s="2">
-        <f>J14/E14</f>
+        <f t="shared" si="3"/>
         <v>10.833333333333334</v>
       </c>
       <c r="L14" s="13">
@@ -2441,17 +2387,14 @@
         <v>1</v>
       </c>
       <c r="N14" s="17">
-        <f>IF(L14&lt;1,(J14+$B$49)/E14,K14)</f>
+        <f t="shared" si="4"/>
         <v>10.833333333333334</v>
       </c>
       <c r="O14">
         <v>1</v>
       </c>
       <c r="P14" s="17">
-        <f>(J14
-+(IF(L14&lt;1,esta,0)
-+(O14-1)*amob))
-/E14</f>
+        <f t="shared" si="5"/>
         <v>10.833333333333334</v>
       </c>
       <c r="Q14" s="5"/>
@@ -2462,11 +2405,7 @@
         <v>2</v>
       </c>
       <c r="T14" s="17">
-        <f>(J14
-+(IF(L14&lt;1,esta,0)
-+(O14-1)*amob)
-+(S14-1)*este)
-/E14</f>
+        <f t="shared" si="6"/>
         <v>11.354166666666666</v>
       </c>
       <c r="U14" s="6"/>
@@ -2480,18 +2419,18 @@
       <c r="AC14" s="6"/>
       <c r="AD14" s="13"/>
       <c r="AG14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AH14" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AI14" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A15" s="10">
-        <f>A14+1</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="B15" s="32" t="s">
@@ -2504,7 +2443,7 @@
         <v>1</v>
       </c>
       <c r="E15" s="7">
-        <f>IF(G15&lt;&gt;"",G15,F15)</f>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="F15" s="7">
@@ -2520,11 +2459,11 @@
         <v>60</v>
       </c>
       <c r="J15" s="7">
-        <f>H15+I15</f>
+        <f t="shared" si="2"/>
         <v>440</v>
       </c>
       <c r="K15" s="8">
-        <f>J15/E15</f>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="L15" s="13">
@@ -2534,48 +2473,41 @@
         <v>1</v>
       </c>
       <c r="N15" s="17">
-        <f>IF(L15&lt;1,(J15+$B$49)/E15,K15)</f>
+        <f t="shared" si="4"/>
         <v>11</v>
       </c>
       <c r="O15">
         <v>1</v>
       </c>
       <c r="P15" s="17">
-        <f>(J15
-+(IF(L15&lt;1,esta,0)
-+(O15-1)*amob))
-/E15</f>
+        <f t="shared" si="5"/>
         <v>11</v>
       </c>
       <c r="S15" s="13">
         <v>2</v>
       </c>
       <c r="T15" s="17">
-        <f>(J15
-+(IF(L15&lt;1,esta,0)
-+(O15-1)*amob)
-+(S15-1)*este)
-/E15</f>
+        <f t="shared" si="6"/>
         <v>11.625</v>
       </c>
       <c r="AD15" s="13"/>
       <c r="AG15" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AH15" t="s">
+        <v>110</v>
+      </c>
+      <c r="AI15" s="1" t="s">
         <v>111</v>
-      </c>
-      <c r="AI15" s="1" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="16" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A16" s="10">
-        <f>A15+1</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -2584,7 +2516,7 @@
         <v>1</v>
       </c>
       <c r="E16">
-        <f>IF(G16&lt;&gt;"",G16,F16)</f>
+        <f t="shared" si="1"/>
         <v>43</v>
       </c>
       <c r="F16">
@@ -2600,11 +2532,11 @@
         <v>75</v>
       </c>
       <c r="J16">
-        <f>H16+I16</f>
+        <f t="shared" si="2"/>
         <v>495</v>
       </c>
       <c r="K16" s="2">
-        <f>J16/E16</f>
+        <f t="shared" si="3"/>
         <v>11.511627906976743</v>
       </c>
       <c r="L16" s="13">
@@ -2614,17 +2546,14 @@
         <v>1</v>
       </c>
       <c r="N16" s="17">
-        <f>IF(L16&lt;1,(J16+$B$49)/E16,K16)</f>
+        <f t="shared" si="4"/>
         <v>11.511627906976743</v>
       </c>
       <c r="O16">
         <v>1</v>
       </c>
       <c r="P16" s="17">
-        <f>(J16
-+(IF(L16&lt;1,esta,0)
-+(O16-1)*amob))
-/E16</f>
+        <f t="shared" si="5"/>
         <v>11.511627906976743</v>
       </c>
       <c r="Q16" s="5"/>
@@ -2635,11 +2564,7 @@
         <v>2</v>
       </c>
       <c r="T16" s="17">
-        <f>(J16
-+(IF(L16&lt;1,esta,0)
-+(O16-1)*amob)
-+(S16-1)*este)
-/E16</f>
+        <f t="shared" si="6"/>
         <v>12.093023255813954</v>
       </c>
       <c r="U16" s="6"/>
@@ -2653,15 +2578,15 @@
       <c r="AC16" s="6"/>
       <c r="AD16" s="13"/>
       <c r="AG16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AI16" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A17" s="10">
-        <f>A16+1</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="B17" s="3" t="s">
@@ -2674,7 +2599,7 @@
         <v>1</v>
       </c>
       <c r="E17">
-        <f>IF(G17&lt;&gt;"",G17,F17)</f>
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
       <c r="F17">
@@ -2687,11 +2612,11 @@
         <v>80</v>
       </c>
       <c r="J17">
-        <f>H17+I17</f>
+        <f t="shared" si="2"/>
         <v>500</v>
       </c>
       <c r="K17" s="2">
-        <f>J17/E17</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="L17" s="13">
@@ -2701,17 +2626,14 @@
         <v>1</v>
       </c>
       <c r="N17" s="17">
-        <f>IF(L17&lt;1,(J17+$B$49)/E17,K17)</f>
+        <f t="shared" si="4"/>
         <v>11.2</v>
       </c>
       <c r="O17">
         <v>1</v>
       </c>
       <c r="P17" s="17">
-        <f>(J17
-+(IF(L17&lt;1,esta,0)
-+(O17-1)*amob))
-/E17</f>
+        <f t="shared" si="5"/>
         <v>11.2</v>
       </c>
       <c r="Q17" s="5"/>
@@ -2719,11 +2641,7 @@
         <v>3</v>
       </c>
       <c r="T17" s="17">
-        <f>(J17
-+(IF(L17&lt;1,esta,0)
-+(O17-1)*amob)
-+(S17-1)*este)
-/E17</f>
+        <f t="shared" si="6"/>
         <v>12.2</v>
       </c>
       <c r="U17" s="6"/>
@@ -2748,11 +2666,11 @@
     </row>
     <row r="18" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A18" s="10">
-        <f>A17+1</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -2761,7 +2679,7 @@
         <v>1</v>
       </c>
       <c r="E18">
-        <f>IF(G18&lt;&gt;"",G18,F18)</f>
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
       <c r="F18">
@@ -2777,11 +2695,11 @@
         <v>100</v>
       </c>
       <c r="J18">
-        <f>H18+I18</f>
+        <f t="shared" si="2"/>
         <v>500</v>
       </c>
       <c r="K18" s="2">
-        <f>J18/E18</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="L18" s="13">
@@ -2791,17 +2709,14 @@
         <v>0</v>
       </c>
       <c r="N18" s="17">
-        <f>IF(L18&lt;1,(J18+$B$49)/E18,K18)</f>
+        <f t="shared" si="4"/>
         <v>11.2</v>
       </c>
       <c r="O18">
         <v>1</v>
       </c>
       <c r="P18" s="17">
-        <f>(J18
-+(IF(L18&lt;1,esta,0)
-+(O18-1)*amob))
-/E18</f>
+        <f t="shared" si="5"/>
         <v>11.2</v>
       </c>
       <c r="Q18" s="5"/>
@@ -2809,11 +2724,7 @@
         <v>3</v>
       </c>
       <c r="T18" s="17">
-        <f>(J18
-+(IF(L18&lt;1,esta,0)
-+(O18-1)*amob)
-+(S18-1)*este)
-/E18</f>
+        <f t="shared" si="6"/>
         <v>12.2</v>
       </c>
       <c r="U18" s="6"/>
@@ -2827,16 +2738,16 @@
       <c r="AC18" s="6"/>
       <c r="AD18" s="13"/>
       <c r="AG18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A19" s="10">
-        <f>A18+1</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C19" s="5">
         <v>1</v>
@@ -2845,7 +2756,7 @@
         <v>1</v>
       </c>
       <c r="E19" s="5">
-        <f>IF(G19&lt;&gt;"",G19,F19)</f>
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
       <c r="F19" s="5">
@@ -2861,11 +2772,11 @@
         <v>90</v>
       </c>
       <c r="J19" s="5">
-        <f>H19+I19</f>
+        <f t="shared" si="2"/>
         <v>590</v>
       </c>
       <c r="K19" s="6">
-        <f>J19/E19</f>
+        <f t="shared" si="3"/>
         <v>11.8</v>
       </c>
       <c r="L19" s="5">
@@ -2875,17 +2786,14 @@
         <v>0</v>
       </c>
       <c r="N19" s="6">
-        <f>IF(L19&lt;1,(J19+$B$49)/E19,K19)</f>
+        <f t="shared" si="4"/>
         <v>11.8</v>
       </c>
       <c r="O19">
         <v>1</v>
       </c>
       <c r="P19" s="6">
-        <f>(J19
-+(IF(L19&lt;1,esta,0)
-+(O19-1)*amob))
-/E19</f>
+        <f t="shared" si="5"/>
         <v>11.8</v>
       </c>
       <c r="Q19" s="5"/>
@@ -2896,22 +2804,18 @@
         <v>2</v>
       </c>
       <c r="T19" s="6">
-        <f>(J19
-+(IF(L19&lt;1,esta,0)
-+(O19-1)*amob)
-+(S19-1)*este)
-/E19</f>
+        <f t="shared" si="6"/>
         <v>12.3</v>
       </c>
       <c r="U19" s="6"/>
       <c r="V19" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="W19" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="W19" s="2" t="s">
-        <v>107</v>
-      </c>
       <c r="X19" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="Y19" s="6"/>
       <c r="Z19" s="6"/>
@@ -2920,23 +2824,23 @@
       <c r="AC19" s="6"/>
       <c r="AD19" s="13"/>
       <c r="AF19" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="AG19" s="5" t="s">
         <v>74</v>
-      </c>
-      <c r="AG19" s="5" t="s">
-        <v>75</v>
       </c>
       <c r="AH19" s="5"/>
       <c r="AI19" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="20" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A20" s="10">
-        <f>A19+1</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C20" s="5">
         <v>1</v>
@@ -2945,7 +2849,7 @@
         <v>1</v>
       </c>
       <c r="E20" s="5">
-        <f>IF(G20&lt;&gt;"",G20,F20)</f>
+        <f t="shared" si="1"/>
         <v>42</v>
       </c>
       <c r="F20" s="5"/>
@@ -2957,11 +2861,11 @@
       </c>
       <c r="I20" s="5"/>
       <c r="J20" s="5">
-        <f>H20+I20</f>
+        <f t="shared" si="2"/>
         <v>435</v>
       </c>
       <c r="K20" s="6">
-        <f>J20/E20</f>
+        <f t="shared" si="3"/>
         <v>10.357142857142858</v>
       </c>
       <c r="L20" s="13">
@@ -2971,32 +2875,25 @@
         <v>0</v>
       </c>
       <c r="N20" s="17">
-        <f>IF(L20&lt;1,(J20+$B$49)/E20,K20)</f>
+        <f t="shared" si="4"/>
         <v>11.785714285714286</v>
       </c>
       <c r="O20" s="5">
         <v>1</v>
       </c>
       <c r="P20" s="17">
-        <f>(J20
-+(IF(L20&lt;1,esta,0)
-+(O20-1)*amob))
-/E20</f>
+        <f t="shared" si="5"/>
         <v>11.785714285714286</v>
       </c>
       <c r="Q20" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="R20" s="5"/>
       <c r="S20" s="13">
         <v>2</v>
       </c>
       <c r="T20" s="17">
-        <f>(J20
-+(IF(L20&lt;1,esta,0)
-+(O20-1)*amob)
-+(S20-1)*este)
-/E20</f>
+        <f t="shared" si="6"/>
         <v>12.380952380952381</v>
       </c>
       <c r="U20" s="6"/>
@@ -3010,22 +2907,22 @@
       <c r="AC20" s="6"/>
       <c r="AD20" s="13"/>
       <c r="AF20" t="s">
+        <v>40</v>
+      </c>
+      <c r="AG20" t="s">
+        <v>31</v>
+      </c>
+      <c r="AI20" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="AG20" t="s">
-        <v>32</v>
-      </c>
-      <c r="AI20" s="1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A21" s="10">
-        <f>A20+1</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C21" s="7">
         <v>1</v>
@@ -3034,7 +2931,7 @@
         <v>1</v>
       </c>
       <c r="E21" s="7">
-        <f>IF(G21&lt;&gt;"",G21,F21)</f>
+        <f t="shared" si="1"/>
         <v>46</v>
       </c>
       <c r="F21" s="7">
@@ -3050,11 +2947,11 @@
         <v>95</v>
       </c>
       <c r="J21" s="7">
-        <f>H21+I21</f>
+        <f t="shared" si="2"/>
         <v>495</v>
       </c>
       <c r="K21" s="8">
-        <f>J21/E21</f>
+        <f t="shared" si="3"/>
         <v>10.760869565217391</v>
       </c>
       <c r="L21" s="13">
@@ -3064,48 +2961,41 @@
         <v>1</v>
       </c>
       <c r="N21" s="17">
-        <f>IF(L21&lt;1,(J21+$B$49)/E21,K21)</f>
+        <f t="shared" si="4"/>
         <v>10.760869565217391</v>
       </c>
       <c r="O21">
         <v>2</v>
       </c>
       <c r="P21" s="17">
-        <f>(J21
-+(IF(L21&lt;1,esta,0)
-+(O21-1)*amob))
-/E21</f>
+        <f t="shared" si="5"/>
         <v>11.485507246376812</v>
       </c>
       <c r="S21" s="13">
         <v>3</v>
       </c>
       <c r="T21" s="17">
-        <f>(J21
-+(IF(L21&lt;1,esta,0)
-+(O21-1)*amob)
-+(S21-1)*este)
-/E21</f>
+        <f t="shared" si="6"/>
         <v>12.572463768115943</v>
       </c>
       <c r="AD21" s="13"/>
       <c r="AG21" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AH21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AI21" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="22" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A22" s="10">
-        <f>A21+1</f>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C22" s="7">
         <v>1</v>
@@ -3114,7 +3004,7 @@
         <v>1</v>
       </c>
       <c r="E22" s="7">
-        <f>IF(G22&lt;&gt;"",G22,F22)</f>
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
       <c r="F22" s="7">
@@ -3130,11 +3020,11 @@
         <v>120</v>
       </c>
       <c r="J22" s="7">
-        <f>H22+I22</f>
+        <f t="shared" si="2"/>
         <v>520</v>
       </c>
       <c r="K22" s="8">
-        <f>J22/E22</f>
+        <f t="shared" si="3"/>
         <v>10.4</v>
       </c>
       <c r="L22" s="13">
@@ -3144,48 +3034,41 @@
         <v>0</v>
       </c>
       <c r="N22" s="17">
-        <f>IF(L22&lt;1,(J22+$B$49)/E22,K22)</f>
+        <f t="shared" si="4"/>
         <v>11.6</v>
       </c>
       <c r="O22">
         <v>1</v>
       </c>
       <c r="P22" s="17">
-        <f>(J22
-+(IF(L22&lt;1,esta,0)
-+(O22-1)*amob))
-/E22</f>
+        <f t="shared" si="5"/>
         <v>11.6</v>
       </c>
       <c r="S22" s="13">
         <v>3</v>
       </c>
       <c r="T22" s="17">
-        <f>(J22
-+(IF(L22&lt;1,esta,0)
-+(O22-1)*amob)
-+(S22-1)*este)
-/E22</f>
+        <f t="shared" si="6"/>
         <v>12.6</v>
       </c>
       <c r="AD22" s="13"/>
       <c r="AG22" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AH22" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="AI22" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="23" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A23" s="10">
-        <f>A22+1</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C23" s="5">
         <v>1</v>
@@ -3194,7 +3077,7 @@
         <v>1</v>
       </c>
       <c r="E23" s="5">
-        <f>IF(G23&lt;&gt;"",G23,F23)</f>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="F23" s="5">
@@ -3210,11 +3093,11 @@
         <v>75</v>
       </c>
       <c r="J23" s="5">
-        <f>H23+I23</f>
+        <f t="shared" si="2"/>
         <v>455</v>
       </c>
       <c r="K23" s="6">
-        <f>J23/E23</f>
+        <f t="shared" si="3"/>
         <v>11.375</v>
       </c>
       <c r="L23" s="13">
@@ -3224,17 +3107,14 @@
         <v>1</v>
       </c>
       <c r="N23" s="17">
-        <f>IF(L23&lt;1,(J23+$B$49)/E23,K23)</f>
+        <f t="shared" si="4"/>
         <v>11.375</v>
       </c>
       <c r="O23" s="5">
         <v>1</v>
       </c>
       <c r="P23" s="17">
-        <f>(J23
-+(IF(L23&lt;1,esta,0)
-+(O23-1)*amob))
-/E23</f>
+        <f t="shared" si="5"/>
         <v>11.375</v>
       </c>
       <c r="Q23" s="5"/>
@@ -3243,11 +3123,7 @@
         <v>3</v>
       </c>
       <c r="T23" s="17">
-        <f>(J23
-+(IF(L23&lt;1,esta,0)
-+(O23-1)*amob)
-+(S23-1)*este)
-/E23</f>
+        <f t="shared" si="6"/>
         <v>12.625</v>
       </c>
       <c r="U23" s="6"/>
@@ -3261,19 +3137,19 @@
       <c r="AC23" s="6"/>
       <c r="AD23" s="13"/>
       <c r="AG23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AI23" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="24" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A24" s="10">
-        <f>A23+1</f>
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C24" s="7">
         <v>1</v>
@@ -3282,7 +3158,7 @@
         <v>1</v>
       </c>
       <c r="E24" s="7">
-        <f>IF(G24&lt;&gt;"",G24,F24)</f>
+        <f t="shared" si="1"/>
         <v>45</v>
       </c>
       <c r="F24" s="7">
@@ -3298,11 +3174,11 @@
         <v>60</v>
       </c>
       <c r="J24" s="7">
-        <f>H24+I24</f>
+        <f t="shared" si="2"/>
         <v>490</v>
       </c>
       <c r="K24" s="8">
-        <f>J24/E24</f>
+        <f t="shared" si="3"/>
         <v>10.888888888888889</v>
       </c>
       <c r="L24" s="13">
@@ -3312,17 +3188,14 @@
         <v>0</v>
       </c>
       <c r="N24" s="17">
-        <f>IF(L24&lt;1,(J24+$B$49)/E24,K24)</f>
+        <f t="shared" si="4"/>
         <v>12.222222222222221</v>
       </c>
       <c r="O24">
         <v>1</v>
       </c>
       <c r="P24" s="17">
-        <f>(J24
-+(IF(L24&lt;1,esta,0)
-+(O24-1)*amob))
-/E24</f>
+        <f t="shared" si="5"/>
         <v>12.222222222222221</v>
       </c>
       <c r="R24">
@@ -3332,28 +3205,24 @@
         <v>2</v>
       </c>
       <c r="T24" s="17">
-        <f>(J24
-+(IF(L24&lt;1,esta,0)
-+(O24-1)*amob)
-+(S24-1)*este)
-/E24</f>
+        <f t="shared" si="6"/>
         <v>12.777777777777779</v>
       </c>
       <c r="AD24" s="13"/>
       <c r="AH24" t="s">
+        <v>116</v>
+      </c>
+      <c r="AI24" s="1" t="s">
         <v>117</v>
-      </c>
-      <c r="AI24" s="1" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="25" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A25" s="10">
-        <f>A24+1</f>
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C25" s="7">
         <v>1</v>
@@ -3362,7 +3231,7 @@
         <v>1</v>
       </c>
       <c r="E25" s="7">
-        <f>IF(G25&lt;&gt;"",G25,F25)</f>
+        <f t="shared" si="1"/>
         <v>45</v>
       </c>
       <c r="F25" s="7">
@@ -3378,11 +3247,11 @@
         <v>110</v>
       </c>
       <c r="J25" s="7">
-        <f>H25+I25</f>
+        <f t="shared" si="2"/>
         <v>560</v>
       </c>
       <c r="K25" s="8">
-        <f>J25/E25</f>
+        <f t="shared" si="3"/>
         <v>12.444444444444445</v>
       </c>
       <c r="L25" s="14">
@@ -3392,17 +3261,14 @@
         <v>1</v>
       </c>
       <c r="N25" s="17">
-        <f>IF(L25&lt;1,(J25+$B$49)/E25,K25)</f>
+        <f t="shared" si="4"/>
         <v>12.444444444444445</v>
       </c>
       <c r="O25">
         <v>1</v>
       </c>
       <c r="P25" s="17">
-        <f>(J25
-+(IF(L25&lt;1,esta,0)
-+(O25-1)*amob))
-/E25</f>
+        <f t="shared" si="5"/>
         <v>12.444444444444445</v>
       </c>
       <c r="Q25" s="5"/>
@@ -3413,11 +3279,7 @@
         <v>2</v>
       </c>
       <c r="T25" s="17">
-        <f>(J25
-+(IF(L25&lt;1,esta,0)
-+(O25-1)*amob)
-+(S25-1)*este)
-/E25</f>
+        <f t="shared" si="6"/>
         <v>13</v>
       </c>
       <c r="U25" s="6"/>
@@ -3436,11 +3298,11 @@
     </row>
     <row r="26" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A26" s="10">
-        <f>A25+1</f>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -3449,7 +3311,7 @@
         <v>1</v>
       </c>
       <c r="E26">
-        <f>IF(G26&lt;&gt;"",G26,F26)</f>
+        <f t="shared" si="1"/>
         <v>42</v>
       </c>
       <c r="F26">
@@ -3465,11 +3327,11 @@
         <v>75</v>
       </c>
       <c r="J26">
-        <f>H26+I26</f>
+        <f t="shared" si="2"/>
         <v>525</v>
       </c>
       <c r="K26" s="2">
-        <f>J26/E26</f>
+        <f t="shared" si="3"/>
         <v>12.5</v>
       </c>
       <c r="L26" s="13">
@@ -3479,17 +3341,14 @@
         <v>1</v>
       </c>
       <c r="N26" s="17">
-        <f>IF(L26&lt;1,(J26+$B$49)/E26,K26)</f>
+        <f t="shared" si="4"/>
         <v>12.5</v>
       </c>
       <c r="O26">
         <v>1</v>
       </c>
       <c r="P26" s="17">
-        <f>(J26
-+(IF(L26&lt;1,esta,0)
-+(O26-1)*amob))
-/E26</f>
+        <f t="shared" si="5"/>
         <v>12.5</v>
       </c>
       <c r="Q26" s="5"/>
@@ -3500,11 +3359,7 @@
         <v>2</v>
       </c>
       <c r="T26" s="17">
-        <f>(J26
-+(IF(L26&lt;1,esta,0)
-+(O26-1)*amob)
-+(S26-1)*este)
-/E26</f>
+        <f t="shared" si="6"/>
         <v>13.095238095238095</v>
       </c>
       <c r="U26" s="6"/>
@@ -3518,15 +3373,15 @@
       <c r="AC26" s="6"/>
       <c r="AD26" s="13"/>
       <c r="AG26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AI26" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="27" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A27" s="10">
-        <f>A26+1</f>
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="B27" s="3" t="s">
@@ -3539,7 +3394,7 @@
         <v>1</v>
       </c>
       <c r="E27">
-        <f>IF(G27&lt;&gt;"",G27,F27)</f>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="F27">
@@ -3555,11 +3410,11 @@
         <v>50</v>
       </c>
       <c r="J27">
-        <f>H27+I27</f>
+        <f t="shared" si="2"/>
         <v>490</v>
       </c>
       <c r="K27" s="2">
-        <f>J27/E27</f>
+        <f t="shared" si="3"/>
         <v>12.25</v>
       </c>
       <c r="L27" s="13">
@@ -3569,17 +3424,14 @@
         <v>1</v>
       </c>
       <c r="N27" s="17">
-        <f>IF(L27&lt;1,(J27+$B$49)/E27,K27)</f>
+        <f t="shared" si="4"/>
         <v>12.25</v>
       </c>
       <c r="O27">
         <v>1</v>
       </c>
       <c r="P27" s="17">
-        <f>(J27
-+(IF(L27&lt;1,esta,0)
-+(O27-1)*amob))
-/E27</f>
+        <f t="shared" si="5"/>
         <v>12.25</v>
       </c>
       <c r="Q27" s="5"/>
@@ -3587,11 +3439,7 @@
         <v>2.5</v>
       </c>
       <c r="T27" s="17">
-        <f>(J27
-+(IF(L27&lt;1,esta,0)
-+(O27-1)*amob)
-+(S27-1)*este)
-/E27</f>
+        <f t="shared" si="6"/>
         <v>13.1875</v>
       </c>
       <c r="U27" s="6"/>
@@ -3605,7 +3453,7 @@
       <c r="AC27" s="6"/>
       <c r="AD27" s="13"/>
       <c r="AG27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AI27" s="1" t="s">
         <v>20</v>
@@ -3613,11 +3461,11 @@
     </row>
     <row r="28" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A28" s="10">
-        <f>A27+1</f>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="B28" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -3626,7 +3474,7 @@
         <v>1</v>
       </c>
       <c r="E28">
-        <f>IF(G28&lt;&gt;"",G28,F28)</f>
+        <f t="shared" si="1"/>
         <v>45</v>
       </c>
       <c r="F28">
@@ -3642,11 +3490,11 @@
         <v>120</v>
       </c>
       <c r="J28">
-        <f>H28+I28</f>
+        <f t="shared" si="2"/>
         <v>520</v>
       </c>
       <c r="K28" s="2">
-        <f>J28/E28</f>
+        <f t="shared" si="3"/>
         <v>11.555555555555555</v>
       </c>
       <c r="L28" s="13">
@@ -3656,17 +3504,14 @@
         <v>1</v>
       </c>
       <c r="N28" s="17">
-        <f>IF(L28&lt;1,(J28+$B$49)/E28,K28)</f>
+        <f t="shared" si="4"/>
         <v>11.555555555555555</v>
       </c>
       <c r="O28">
         <v>1</v>
       </c>
       <c r="P28" s="17">
-        <f>(J28
-+(IF(L28&lt;1,esta,0)
-+(O28-1)*amob))
-/E28</f>
+        <f t="shared" si="5"/>
         <v>11.555555555555555</v>
       </c>
       <c r="Q28" s="5"/>
@@ -3674,11 +3519,7 @@
         <v>4</v>
       </c>
       <c r="T28" s="17">
-        <f>(J28
-+(IF(L28&lt;1,esta,0)
-+(O28-1)*amob)
-+(S28-1)*este)
-/E28</f>
+        <f t="shared" si="6"/>
         <v>13.222222222222221</v>
       </c>
       <c r="U28" s="6"/>
@@ -3692,19 +3533,19 @@
       <c r="AC28" s="6"/>
       <c r="AD28" s="13"/>
       <c r="AG28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AI28" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="29" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A29" s="10">
-        <f>A28+1</f>
+        <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C29" s="7">
         <v>1</v>
@@ -3713,7 +3554,7 @@
         <v>1</v>
       </c>
       <c r="E29" s="7">
-        <f>IF(G29&lt;&gt;"",G29,F29)</f>
+        <f t="shared" si="1"/>
         <v>45</v>
       </c>
       <c r="F29" s="7">
@@ -3729,11 +3570,11 @@
         <v>100</v>
       </c>
       <c r="J29" s="7">
-        <f>H29+I29</f>
+        <f t="shared" si="2"/>
         <v>490</v>
       </c>
       <c r="K29" s="8">
-        <f>J29/E29</f>
+        <f t="shared" si="3"/>
         <v>10.888888888888889</v>
       </c>
       <c r="L29" s="13">
@@ -3743,48 +3584,41 @@
         <v>1</v>
       </c>
       <c r="N29" s="17">
-        <f>IF(L29&lt;1,(J29+$B$49)/E29,K29)</f>
+        <f t="shared" si="4"/>
         <v>12.222222222222221</v>
       </c>
       <c r="O29">
         <v>1</v>
       </c>
       <c r="P29" s="17">
-        <f>(J29
-+(IF(L29&lt;1,esta,0)
-+(O29-1)*amob))
-/E29</f>
+        <f t="shared" si="5"/>
         <v>12.222222222222221</v>
       </c>
       <c r="S29" s="13">
         <v>3</v>
       </c>
       <c r="T29" s="17">
-        <f>(J29
-+(IF(L29&lt;1,esta,0)
-+(O29-1)*amob)
-+(S29-1)*este)
-/E29</f>
+        <f t="shared" si="6"/>
         <v>13.333333333333334</v>
       </c>
       <c r="AD29" s="13"/>
       <c r="AG29" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AH29" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AI29" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="30" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A30" s="10">
-        <f>A29+1</f>
+        <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C30">
         <v>1</v>
@@ -3793,7 +3627,7 @@
         <v>1</v>
       </c>
       <c r="E30">
-        <f>IF(G30&lt;&gt;"",G30,F30)</f>
+        <f t="shared" si="1"/>
         <v>45</v>
       </c>
       <c r="F30">
@@ -3809,11 +3643,11 @@
         <v>100</v>
       </c>
       <c r="J30">
-        <f>H30+I30</f>
+        <f t="shared" si="2"/>
         <v>535</v>
       </c>
       <c r="K30" s="2">
-        <f>J30/E30</f>
+        <f t="shared" si="3"/>
         <v>11.888888888888889</v>
       </c>
       <c r="L30" s="13">
@@ -3823,17 +3657,14 @@
         <v>1</v>
       </c>
       <c r="N30" s="17">
-        <f>IF(L30&lt;1,(J30+$B$49)/E30,K30)</f>
+        <f t="shared" si="4"/>
         <v>13.222222222222221</v>
       </c>
       <c r="O30">
         <v>1</v>
       </c>
       <c r="P30" s="17">
-        <f>(J30
-+(IF(L30&lt;1,esta,0)
-+(O30-1)*amob))
-/E30</f>
+        <f t="shared" si="5"/>
         <v>13.222222222222221</v>
       </c>
       <c r="Q30" s="5"/>
@@ -3844,11 +3675,7 @@
         <v>2</v>
       </c>
       <c r="T30" s="17">
-        <f>(J30
-+(IF(L30&lt;1,esta,0)
-+(O30-1)*amob)
-+(S30-1)*este)
-/E30</f>
+        <f t="shared" si="6"/>
         <v>13.777777777777779</v>
       </c>
       <c r="U30" s="6"/>
@@ -3862,15 +3689,15 @@
       <c r="AC30" s="6"/>
       <c r="AD30" s="13"/>
       <c r="AG30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AI30" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="31" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A31" s="10">
-        <f>A30+1</f>
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="B31" s="3" t="s">
@@ -3883,7 +3710,7 @@
         <v>1</v>
       </c>
       <c r="E31">
-        <f>IF(G31&lt;&gt;"",G31,F31)</f>
+        <f t="shared" si="1"/>
         <v>49</v>
       </c>
       <c r="F31">
@@ -3899,11 +3726,11 @@
         <v>120</v>
       </c>
       <c r="J31">
-        <f>H31+I31</f>
+        <f t="shared" si="2"/>
         <v>570</v>
       </c>
       <c r="K31" s="2">
-        <f>J31/E31</f>
+        <f t="shared" si="3"/>
         <v>11.63265306122449</v>
       </c>
       <c r="L31" s="13">
@@ -3913,17 +3740,14 @@
         <v>1</v>
       </c>
       <c r="N31" s="17">
-        <f>IF(L31&lt;1,(J31+$B$49)/E31,K31)</f>
+        <f t="shared" si="4"/>
         <v>12.857142857142858</v>
       </c>
       <c r="O31">
         <v>1</v>
       </c>
       <c r="P31" s="17">
-        <f>(J31
-+(IF(L31&lt;1,esta,0)
-+(O31-1)*amob))
-/E31</f>
+        <f t="shared" si="5"/>
         <v>12.857142857142858</v>
       </c>
       <c r="Q31" s="5"/>
@@ -3931,11 +3755,7 @@
         <v>3</v>
       </c>
       <c r="T31" s="17">
-        <f>(J31
-+(IF(L31&lt;1,esta,0)
-+(O31-1)*amob)
-+(S31-1)*este)
-/E31</f>
+        <f t="shared" si="6"/>
         <v>13.877551020408163</v>
       </c>
       <c r="U31" s="6"/>
@@ -3949,19 +3769,19 @@
       <c r="AC31" s="6"/>
       <c r="AD31" s="13"/>
       <c r="AG31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AI31" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="32" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A32" s="10">
-        <f>A31+1</f>
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -3970,7 +3790,7 @@
         <v>1</v>
       </c>
       <c r="E32">
-        <f>IF(G32&lt;&gt;"",G32,F32)</f>
+        <f t="shared" si="1"/>
         <v>45</v>
       </c>
       <c r="F32">
@@ -3986,11 +3806,11 @@
         <v>120</v>
       </c>
       <c r="J32">
-        <f>H32+I32</f>
+        <f t="shared" si="2"/>
         <v>520</v>
       </c>
       <c r="K32" s="2">
-        <f>J32/E32</f>
+        <f t="shared" si="3"/>
         <v>11.555555555555555</v>
       </c>
       <c r="L32" s="13">
@@ -4000,17 +3820,14 @@
         <v>0</v>
       </c>
       <c r="N32" s="17">
-        <f>IF(L32&lt;1,(J32+$B$49)/E32,K32)</f>
+        <f t="shared" si="4"/>
         <v>12.888888888888889</v>
       </c>
       <c r="O32">
         <v>1</v>
       </c>
       <c r="P32" s="17">
-        <f>(J32
-+(IF(L32&lt;1,esta,0)
-+(O32-1)*amob))
-/E32</f>
+        <f t="shared" si="5"/>
         <v>12.888888888888889</v>
       </c>
       <c r="Q32" s="5"/>
@@ -4018,11 +3835,7 @@
         <v>3</v>
       </c>
       <c r="T32" s="17">
-        <f>(J32
-+(IF(L32&lt;1,esta,0)
-+(O32-1)*amob)
-+(S32-1)*este)
-/E32</f>
+        <f t="shared" si="6"/>
         <v>14</v>
       </c>
       <c r="U32" s="6"/>
@@ -4036,22 +3849,22 @@
       <c r="AC32" s="6"/>
       <c r="AD32" s="13"/>
       <c r="AF32" t="s">
+        <v>51</v>
+      </c>
+      <c r="AG32" t="s">
+        <v>31</v>
+      </c>
+      <c r="AI32" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="AG32" t="s">
-        <v>32</v>
-      </c>
-      <c r="AI32" s="1" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="33" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A33" s="10">
-        <f>A32+1</f>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C33" s="7">
         <v>1</v>
@@ -4060,7 +3873,7 @@
         <v>1</v>
       </c>
       <c r="E33" s="7">
-        <f>IF(G33&lt;&gt;"",G33,F33)</f>
+        <f t="shared" si="1"/>
         <v>42</v>
       </c>
       <c r="F33" s="7">
@@ -4076,11 +3889,11 @@
         <v>60</v>
       </c>
       <c r="J33" s="7">
-        <f>H33+I33</f>
+        <f t="shared" si="2"/>
         <v>480</v>
       </c>
       <c r="K33" s="8">
-        <f>J33/E33</f>
+        <f t="shared" si="3"/>
         <v>11.428571428571429</v>
       </c>
       <c r="L33" s="14">
@@ -4090,17 +3903,14 @@
         <v>0</v>
       </c>
       <c r="N33" s="17">
-        <f>IF(L33&lt;1,(J33+$B$49)/E33,K33)</f>
+        <f t="shared" si="4"/>
         <v>12.857142857142858</v>
       </c>
       <c r="O33">
         <v>1</v>
       </c>
       <c r="P33" s="17">
-        <f>(J33
-+(IF(L33&lt;1,esta,0)
-+(O33-1)*amob))
-/E33</f>
+        <f t="shared" si="5"/>
         <v>12.857142857142858</v>
       </c>
       <c r="Q33" s="5"/>
@@ -4108,11 +3918,7 @@
         <v>3</v>
       </c>
       <c r="T33" s="17">
-        <f>(J33
-+(IF(L33&lt;1,esta,0)
-+(O33-1)*amob)
-+(S33-1)*este)
-/E33</f>
+        <f t="shared" si="6"/>
         <v>14.047619047619047</v>
       </c>
       <c r="U33" s="6"/>
@@ -4131,7 +3937,7 @@
     </row>
     <row r="34" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A34" s="10">
-        <f>A33+1</f>
+        <f t="shared" si="0"/>
         <v>31</v>
       </c>
       <c r="B34" s="3" t="s">
@@ -4144,7 +3950,7 @@
         <v>1</v>
       </c>
       <c r="E34">
-        <f>IF(G34&lt;&gt;"",G34,F34)</f>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="F34">
@@ -4160,11 +3966,11 @@
         <v>50</v>
       </c>
       <c r="J34">
-        <f>H34+I34</f>
+        <f t="shared" si="2"/>
         <v>450</v>
       </c>
       <c r="K34" s="2">
-        <f>J34/E34</f>
+        <f t="shared" si="3"/>
         <v>11.25</v>
       </c>
       <c r="L34" s="13">
@@ -4174,17 +3980,14 @@
         <v>1</v>
       </c>
       <c r="N34" s="17">
-        <f>IF(L34&lt;1,(J34+$B$49)/E34,K34)</f>
+        <f t="shared" si="4"/>
         <v>11.25</v>
       </c>
       <c r="O34">
         <v>3</v>
       </c>
       <c r="P34" s="17">
-        <f>(J34
-+(IF(L34&lt;1,esta,0)
-+(O34-1)*amob))
-/E34</f>
+        <f t="shared" si="5"/>
         <v>12.916666666666666</v>
       </c>
       <c r="Q34" s="5"/>
@@ -4192,11 +3995,7 @@
         <v>3</v>
       </c>
       <c r="T34" s="17">
-        <f>(J34
-+(IF(L34&lt;1,esta,0)
-+(O34-1)*amob)
-+(S34-1)*este)
-/E34</f>
+        <f t="shared" si="6"/>
         <v>14.166666666666666</v>
       </c>
       <c r="U34" s="6"/>
@@ -4210,22 +4009,22 @@
       <c r="AC34" s="6"/>
       <c r="AD34" s="5"/>
       <c r="AF34" t="s">
+        <v>35</v>
+      </c>
+      <c r="AG34" t="s">
+        <v>31</v>
+      </c>
+      <c r="AI34" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="AG34" t="s">
-        <v>32</v>
-      </c>
-      <c r="AI34" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="35" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A35" s="10">
-        <f>A34+1</f>
+        <f t="shared" si="0"/>
         <v>32</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C35">
         <v>1</v>
@@ -4234,7 +4033,7 @@
         <v>1</v>
       </c>
       <c r="E35">
-        <f>IF(G35&lt;&gt;"",G35,F35)</f>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="F35">
@@ -4250,11 +4049,11 @@
         <v>68</v>
       </c>
       <c r="J35">
-        <f>H35+I35</f>
+        <f t="shared" si="2"/>
         <v>488</v>
       </c>
       <c r="K35" s="2">
-        <f>J35/E35</f>
+        <f t="shared" si="3"/>
         <v>12.2</v>
       </c>
       <c r="L35" s="13">
@@ -4264,17 +4063,14 @@
         <v>1</v>
       </c>
       <c r="N35" s="17">
-        <f>IF(L35&lt;1,(J35+$B$49)/E35,K35)</f>
+        <f t="shared" si="4"/>
         <v>13.7</v>
       </c>
       <c r="O35">
         <v>1</v>
       </c>
       <c r="P35" s="17">
-        <f>(J35
-+(IF(L35&lt;1,esta,0)
-+(O35-1)*amob))
-/E35</f>
+        <f t="shared" si="5"/>
         <v>13.7</v>
       </c>
       <c r="Q35" s="5"/>
@@ -4285,11 +4081,7 @@
         <v>2</v>
       </c>
       <c r="T35" s="17">
-        <f>(J35
-+(IF(L35&lt;1,esta,0)
-+(O35-1)*amob)
-+(S35-1)*este)
-/E35</f>
+        <f t="shared" si="6"/>
         <v>14.324999999999999</v>
       </c>
       <c r="U35" s="6"/>
@@ -4303,15 +4095,15 @@
       <c r="AC35" s="6"/>
       <c r="AD35" s="5"/>
       <c r="AG35" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AI35" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="36" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A36" s="10">
-        <f>A35+1</f>
+        <f t="shared" si="0"/>
         <v>33</v>
       </c>
       <c r="B36" s="3" t="s">
@@ -4324,7 +4116,7 @@
         <v>1</v>
       </c>
       <c r="E36">
-        <f>IF(G36&lt;&gt;"",G36,F36)</f>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="F36">
@@ -4344,7 +4136,7 @@
         <v>490</v>
       </c>
       <c r="K36" s="2">
-        <f>J36/E36</f>
+        <f t="shared" si="3"/>
         <v>12.25</v>
       </c>
       <c r="L36" s="13">
@@ -4354,17 +4146,14 @@
         <v>0</v>
       </c>
       <c r="N36" s="17">
-        <f>IF(L36&lt;1,(J36+$B$49)/E36,K36)</f>
+        <f t="shared" si="4"/>
         <v>13.75</v>
       </c>
       <c r="O36">
         <v>1</v>
       </c>
       <c r="P36" s="17">
-        <f>(J36
-+(IF(L36&lt;1,esta,0)
-+(O36-1)*amob))
-/E36</f>
+        <f t="shared" si="5"/>
         <v>13.75</v>
       </c>
       <c r="Q36" s="5"/>
@@ -4372,11 +4161,7 @@
         <v>3</v>
       </c>
       <c r="T36" s="17">
-        <f>(J36
-+(IF(L36&lt;1,esta,0)
-+(O36-1)*amob)
-+(S36-1)*este)
-/E36</f>
+        <f t="shared" si="6"/>
         <v>15</v>
       </c>
       <c r="U36" s="6"/>
@@ -4390,7 +4175,7 @@
       <c r="AC36" s="6"/>
       <c r="AD36" s="5"/>
       <c r="AG36" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AI36" s="1" t="s">
         <v>24</v>
@@ -4398,7 +4183,7 @@
     </row>
     <row r="37" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A37" s="10">
-        <f>A36+1</f>
+        <f t="shared" si="0"/>
         <v>34</v>
       </c>
       <c r="B37" s="3" t="s">
@@ -4411,7 +4196,7 @@
         <v>1</v>
       </c>
       <c r="E37">
-        <f>IF(G37&lt;&gt;"",G37,F37)</f>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="F37">
@@ -4431,7 +4216,7 @@
         <v>535</v>
       </c>
       <c r="K37" s="2">
-        <f>J37/E37</f>
+        <f t="shared" si="3"/>
         <v>13.375</v>
       </c>
       <c r="L37" s="13">
@@ -4441,17 +4226,14 @@
         <v>0</v>
       </c>
       <c r="N37" s="17">
-        <f>IF(L37&lt;1,(J37+$B$49)/E37,K37)</f>
+        <f t="shared" si="4"/>
         <v>14.875</v>
       </c>
       <c r="O37">
         <v>1</v>
       </c>
       <c r="P37" s="17">
-        <f>(J37
-+(IF(L37&lt;1,esta,0)
-+(O37-1)*amob))
-/E37</f>
+        <f t="shared" si="5"/>
         <v>14.875</v>
       </c>
       <c r="Q37" s="5"/>
@@ -4459,11 +4241,7 @@
         <v>3</v>
       </c>
       <c r="T37" s="17">
-        <f>(J37
-+(IF(L37&lt;1,esta,0)
-+(O37-1)*amob)
-+(S37-1)*este)
-/E37</f>
+        <f t="shared" si="6"/>
         <v>16.125</v>
       </c>
       <c r="U37" s="6"/>
@@ -4477,7 +4255,7 @@
       <c r="AC37" s="6"/>
       <c r="AD37" s="5"/>
       <c r="AG37" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AI37" s="1" t="s">
         <v>25</v>
@@ -4485,7 +4263,7 @@
     </row>
     <row r="38" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A38" s="10">
-        <f>A37+1</f>
+        <f t="shared" si="0"/>
         <v>35</v>
       </c>
       <c r="B38" s="7" t="s">
@@ -4498,7 +4276,7 @@
         <v>1</v>
       </c>
       <c r="E38" s="5">
-        <f>IF(G38&lt;&gt;"",G38,F38)</f>
+        <f t="shared" si="1"/>
         <v>36</v>
       </c>
       <c r="F38" s="5">
@@ -4518,7 +4296,7 @@
         <v>480</v>
       </c>
       <c r="K38" s="6">
-        <f>J38/E38</f>
+        <f t="shared" si="3"/>
         <v>13.333333333333334</v>
       </c>
       <c r="L38" s="13">
@@ -4528,17 +4306,14 @@
         <v>0</v>
       </c>
       <c r="N38" s="17">
-        <f>IF(L38&lt;1,(J38+$B$49)/E38,K38)</f>
+        <f t="shared" si="4"/>
         <v>15</v>
       </c>
       <c r="O38">
         <v>1</v>
       </c>
       <c r="P38" s="17">
-        <f>(J38
-+(IF(L38&lt;1,esta,0)
-+(O38-1)*amob))
-/E38</f>
+        <f t="shared" si="5"/>
         <v>15</v>
       </c>
       <c r="Q38" s="5"/>
@@ -4546,11 +4321,7 @@
         <v>3</v>
       </c>
       <c r="T38" s="17">
-        <f>(J38
-+(IF(L38&lt;1,esta,0)
-+(O38-1)*amob)
-+(S38-1)*este)
-/E38</f>
+        <f t="shared" si="6"/>
         <v>16.388888888888889</v>
       </c>
       <c r="U38" s="6"/>
@@ -4565,7 +4336,7 @@
       <c r="AD38" s="5"/>
       <c r="AF38" s="5"/>
       <c r="AG38" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AH38" s="5"/>
       <c r="AI38" s="1" t="s">
@@ -4580,12 +4351,12 @@
     </row>
     <row r="48" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A48" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B49">
         <v>60</v>
@@ -4593,7 +4364,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B50" s="18">
         <f>400/12</f>
@@ -4602,7 +4373,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B51">
         <v>25</v>
@@ -4610,7 +4381,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>